<commit_message>
add results excels files
</commit_message>
<xml_diff>
--- a/total_losses.xlsx
+++ b/total_losses.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afiq Hafizuddin\Documents\MATLAB\01-STATIC-DUMA-AMEND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364F8F4F-5543-4B30-B4BC-77532A73A11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0A30AF-3E89-4E0C-B46C-2FE9B0D9B28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="parallel" sheetId="1" r:id="rId1"/>
+    <sheet name="sectionalized" sheetId="2" r:id="rId2"/>
+    <sheet name="contingency" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>PV Penetration Levels</t>
   </si>
@@ -385,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,4 +476,194 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1EA292-47BC-43A2-AD37-B39DE03D57DC}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="16.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>190.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3">
+        <v>165.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>150</v>
+      </c>
+      <c r="C5" s="3">
+        <v>124.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>200</v>
+      </c>
+      <c r="C6" s="3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>250</v>
+      </c>
+      <c r="C7" s="3">
+        <v>93.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473100CF-B12A-4807-84E8-257D05F97744}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="16.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3">
+        <v>199.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3">
+        <v>173.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>150</v>
+      </c>
+      <c r="C5" s="3">
+        <v>150.30000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>200</v>
+      </c>
+      <c r="C6" s="3">
+        <v>130.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>250</v>
+      </c>
+      <c r="C7" s="3">
+        <v>112.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>